<commit_message>
fixed params, protcols, condition files for andy and steffi
</commit_message>
<xml_diff>
--- a/protocol_steffi_20150814.xlsx
+++ b/protocol_steffi_20150814.xlsx
@@ -144,7 +144,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K29" activeCellId="0" sqref="K29"/>
+      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -194,16 +194,16 @@
         <v>75</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>200</v>
       </c>
       <c r="E2" s="0" t="n">
-        <v>150</v>
+        <v>25</v>
       </c>
       <c r="F2" s="0" t="n">
-        <v>30000</v>
+        <v>60000</v>
       </c>
       <c r="G2" s="0" t="n">
         <v>30</v>
@@ -213,7 +213,7 @@
       </c>
       <c r="I2" s="0" t="n">
         <f aca="false">(D2*E2+F2)*H2+G2*1000</f>
-        <v>330000</v>
+        <v>355000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>